<commit_message>
domain and stats in code-details.xlsx
</commit_message>
<xml_diff>
--- a/Code Label/Code-details.xlsx
+++ b/Code Label/Code-details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S M Kashif\Desktop\research\Self-declare papers\Dataset\Code Label\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S M Kashif\Desktop\research\Self-declare papers\SDAGC-Dataset\Code Label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A908B6B-FF7E-4027-A185-5D16D4C66BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E074772C-5F99-4322-AFFB-B2201333B769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{47953AFF-668F-4BF4-9504-F9DAB3CDE17B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="379">
   <si>
     <t>SR No</t>
   </si>
@@ -967,6 +967,213 @@
   </si>
   <si>
     <t>Contributors</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Code-level Single Instance</t>
+  </si>
+  <si>
+    <t>Source-file level Single Instance</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility tool </t>
+  </si>
+  <si>
+    <t>website &lt;head&gt; content optimzation tool</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>A minimalistic web client</t>
+  </si>
+  <si>
+    <t>Web App</t>
+  </si>
+  <si>
+    <t>Comment Type</t>
+  </si>
+  <si>
+    <t>Self-Declaration Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Real-time locations sharing web app</t>
+  </si>
+  <si>
+    <t>Mentioned ChatGPT</t>
+  </si>
+  <si>
+    <t>Movies Booking Website</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Create Vite-powered vue project</t>
+  </si>
+  <si>
+    <t>DevOps monitoring tool</t>
+  </si>
+  <si>
+    <t>AI software toolkit in the UNIX tradition</t>
+  </si>
+  <si>
+    <t>AI App</t>
+  </si>
+  <si>
+    <t>Discord Bot container</t>
+  </si>
+  <si>
+    <t>Create a module for îles - web generator</t>
+  </si>
+  <si>
+    <t>browser extension</t>
+  </si>
+  <si>
+    <t>Mentioned GitHub Copilot</t>
+  </si>
+  <si>
+    <t>Auto change quotes and image</t>
+  </si>
+  <si>
+    <t>FLoppy Bird game</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> interactive TIC TAC TOE game</t>
+  </si>
+  <si>
+    <t>interactive maze game on a 49x49 grid</t>
+  </si>
+  <si>
+    <t>compiler for new language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A document and inventory tracking software </t>
+  </si>
+  <si>
+    <t>Classroom Monitoring Tool</t>
+  </si>
+  <si>
+    <t>web app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food waste management system </t>
+  </si>
+  <si>
+    <t>System for tracking information about games</t>
+  </si>
+  <si>
+    <t>Not mentioned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep learning package </t>
+  </si>
+  <si>
+    <t>code used to collate and compile food orders</t>
+  </si>
+  <si>
+    <t>Command line tool for Panther rules and policies</t>
+  </si>
+  <si>
+    <t>Source-file level Multiple Instances</t>
+  </si>
+  <si>
+    <t>Convert MythicMob files to Denizen Scripts</t>
+  </si>
+  <si>
+    <t>Deep learning package</t>
+  </si>
+  <si>
+    <t>Code-level Multiple Instances</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>A library of XDE cases and algorithm</t>
+  </si>
+  <si>
+    <t>fake laser simulator to be worked with turtlesim</t>
+  </si>
+  <si>
+    <t>Library  to parse products from bethowen.</t>
+  </si>
+  <si>
+    <t>Puzzles and games</t>
+  </si>
+  <si>
+    <t>Help developers profile their UI thread</t>
+  </si>
+  <si>
+    <t>Demostrate security vulnerabilities</t>
+  </si>
+  <si>
+    <t>Discord Bot made for DCS communities</t>
+  </si>
+  <si>
+    <t>Calculate Hounsfield pixel values from DICOM file</t>
+  </si>
+  <si>
+    <t>Gaming website</t>
+  </si>
+  <si>
+    <t>jMonkeyEngine3 Software Development Kit</t>
+  </si>
+  <si>
+    <t>Extensively customize your character with Figura!</t>
+  </si>
+  <si>
+    <t>Sport tracking application</t>
+  </si>
+  <si>
+    <t>Mobile App</t>
+  </si>
+  <si>
+    <t>Compilers coding</t>
+  </si>
+  <si>
+    <t>Data structures implementation</t>
+  </si>
+  <si>
+    <t>Data-driven interactive timeline</t>
+  </si>
+  <si>
+    <t>Spring-based application with Digma</t>
+  </si>
+  <si>
+    <t>Spring-based application</t>
+  </si>
+  <si>
+    <t>Camunda Platform Process Application</t>
+  </si>
+  <si>
+    <t>transcodes web pages to make them granularly accessible</t>
+  </si>
+  <si>
+    <t>Intellij IDEA plugin to generate Builder pattern code</t>
+  </si>
+  <si>
+    <t>Kaggle and Kaggle API</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Comment Types</t>
+  </si>
+  <si>
+    <t>Self-declaration Type</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1019,8 +1226,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1028,12 +1259,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1056,11 +1302,53 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1397,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{834B8B68-6C12-431F-99D1-DAF8CBABF27C}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,13 +1698,23 @@
     <col min="3" max="3" width="16.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="27.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="31.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" style="1" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="36.77734375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1436,17 +1734,32 @@
         <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1465,14 +1778,29 @@
       <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J2" s="13">
+        <v>2</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="1">
+      <c r="O2" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1491,14 +1819,41 @@
       <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J3" s="13">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="1">
         <v>12</v>
       </c>
-      <c r="H3" s="1">
+      <c r="O3" s="1">
         <v>2503</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q3" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="S3" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="T3" s="22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1517,14 +1872,43 @@
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J4" s="13">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="1">
         <v>2</v>
       </c>
-      <c r="H4" s="1">
+      <c r="O4" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q4" s="10">
+        <v>1</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="S4" s="10">
+        <f>COUNTIF(J2:M51,Q4)</f>
+        <v>28</v>
+      </c>
+      <c r="T4" s="17">
+        <f>SUM(S4,S5)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1543,14 +1927,40 @@
       <c r="F5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="G5" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J5" s="13">
+        <v>2</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q5" s="10">
+        <v>2</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="S5" s="10">
+        <f>COUNTIF(J3:M52,Q5)</f>
+        <v>14</v>
+      </c>
+      <c r="T5" s="17"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1569,14 +1979,43 @@
       <c r="F6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="G6" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J6" s="13">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q6" s="11">
+        <v>3</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="S6" s="11">
+        <f>COUNTIF(J2:M51,Q6)</f>
+        <v>6</v>
+      </c>
+      <c r="T6" s="18">
+        <f>SUM(S6,S7)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1595,14 +2034,40 @@
       <c r="F7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="1">
         <v>2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="O7" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q7" s="11">
+        <v>4</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="S7" s="11">
+        <f>COUNTIF(J3:M52,Q7)</f>
+        <v>4</v>
+      </c>
+      <c r="T7" s="18"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1621,14 +2086,29 @@
       <c r="F8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="G8" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1647,14 +2127,29 @@
       <c r="F9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J9" s="13">
+        <v>1</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="1">
         <v>40</v>
       </c>
-      <c r="H9" s="1">
+      <c r="O9" s="1">
         <v>603</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1673,14 +2168,36 @@
       <c r="F10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J10" s="13">
+        <v>2</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="1">
         <v>5</v>
       </c>
-      <c r="H10" s="1">
+      <c r="O10" s="1">
         <v>1141</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q10" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="R10" s="21"/>
+      <c r="S10" s="22" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1699,14 +2216,39 @@
       <c r="F11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J11" s="13">
+        <v>2</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13">
+        <v>3</v>
+      </c>
+      <c r="M11" s="13"/>
+      <c r="N11" s="1">
         <v>5</v>
       </c>
-      <c r="H11" s="1">
+      <c r="O11" s="1">
         <v>1175</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q11" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="R11" s="16"/>
+      <c r="S11" s="9">
+        <f>COUNTIF(I2:I51,Q11)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1725,14 +2267,37 @@
       <c r="F12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="G12" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J12" s="13">
+        <v>2</v>
+      </c>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
         <v>118</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q12" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="R12" s="16"/>
+      <c r="S12" s="9">
+        <f>COUNTIF(I2:I51,Q12)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1751,14 +2316,37 @@
       <c r="F13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="G13" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J13" s="13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="Q13" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="R13" s="16"/>
+      <c r="S13" s="9">
+        <f>COUNTIF(I2:I51, Q13)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1777,14 +2365,29 @@
       <c r="F14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J14" s="13">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="1">
         <v>2</v>
       </c>
-      <c r="H14" s="1">
+      <c r="O14" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1803,14 +2406,29 @@
       <c r="F15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="G15" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J15" s="13">
+        <v>3</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
         <v>6717</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1829,14 +2447,36 @@
       <c r="F16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="G16" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J16" s="13">
+        <v>1</v>
+      </c>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="1">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="Q16" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="R16" s="23"/>
+      <c r="S16" s="22" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1855,14 +2495,37 @@
       <c r="F17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="G17" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J17" s="13">
+        <v>1</v>
+      </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="1">
+        <v>1</v>
+      </c>
+      <c r="O17" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="Q17" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="R17" s="15"/>
+      <c r="S17" s="12">
+        <f t="shared" ref="S17:S22" si="0">COUNTIF(H2:H51,Q17)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1881,14 +2544,37 @@
       <c r="F18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="G18" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J18" s="13">
+        <v>3</v>
+      </c>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="1">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="Q18" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="R18" s="15"/>
+      <c r="S18" s="12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1907,14 +2593,37 @@
       <c r="F19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
+      <c r="G19" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J19" s="13">
+        <v>1</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="1">
+        <v>1</v>
+      </c>
+      <c r="O19" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="Q19" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="R19" s="15"/>
+      <c r="S19" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1933,14 +2642,37 @@
       <c r="F20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="G20" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J20" s="13">
+        <v>1</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1">
         <v>336</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="Q20" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="R20" s="15"/>
+      <c r="S20" s="12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1959,14 +2691,37 @@
       <c r="F21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J21" s="13">
+        <v>1</v>
+      </c>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="1">
         <v>3</v>
       </c>
-      <c r="H21" s="1">
+      <c r="O21" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="Q21" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="R21" s="15"/>
+      <c r="S21" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1985,14 +2740,37 @@
       <c r="F22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J22" s="13">
+        <v>2</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="1">
         <v>5</v>
       </c>
-      <c r="H22" s="1">
+      <c r="O22" s="1">
         <v>579</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="Q22" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="R22" s="15"/>
+      <c r="S22" s="12">
+        <f>COUNTIF(H7:H51,Q22)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2011,14 +2789,29 @@
       <c r="F23" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J23" s="13">
         <v>2</v>
       </c>
-      <c r="H23" s="1">
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="1">
+        <v>2</v>
+      </c>
+      <c r="O23" s="1">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2037,14 +2830,29 @@
       <c r="F24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="G24" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J24" s="13">
+        <v>2</v>
+      </c>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2063,14 +2871,29 @@
       <c r="F25" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J25" s="13">
+        <v>1</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="1">
         <v>4</v>
       </c>
-      <c r="H25" s="1">
+      <c r="O25" s="1">
         <v>361</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2089,14 +2912,29 @@
       <c r="F26" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J26" s="13">
+        <v>2</v>
+      </c>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="1">
         <v>67</v>
       </c>
-      <c r="H26" s="1">
+      <c r="O26" s="1">
         <v>2501</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2115,14 +2953,29 @@
       <c r="F27" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="G27" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J27" s="13">
+        <v>4</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="1">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2141,14 +2994,31 @@
       <c r="F28" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J28" s="13">
+        <v>2</v>
+      </c>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13">
+        <v>4</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="N28" s="1">
         <v>50</v>
       </c>
-      <c r="H28" s="1">
+      <c r="O28" s="1">
         <v>378</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2167,14 +3037,29 @@
       <c r="F29" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J29" s="13">
+        <v>4</v>
+      </c>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="1">
         <v>15</v>
       </c>
-      <c r="H29" s="1">
+      <c r="O29" s="1">
         <v>927</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2193,14 +3078,29 @@
       <c r="F30" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J30" s="13">
+        <v>1</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="1">
         <v>2</v>
       </c>
-      <c r="H30" s="1">
+      <c r="O30" s="1">
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2219,14 +3119,29 @@
       <c r="F31" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G31" s="1">
-        <v>1</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="G31" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J31" s="13">
+        <v>2</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
         <v>2718</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2245,14 +3160,29 @@
       <c r="F32" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1">
+      <c r="G32" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J32" s="13">
+        <v>1</v>
+      </c>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1">
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2271,14 +3201,29 @@
       <c r="F33" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G33" s="1">
-        <v>1</v>
-      </c>
-      <c r="H33" s="1">
+      <c r="G33" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J33" s="13">
+        <v>1</v>
+      </c>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="1">
+        <v>1</v>
+      </c>
+      <c r="O33" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2297,14 +3242,29 @@
       <c r="F34" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G34" s="1">
-        <v>1</v>
-      </c>
-      <c r="H34" s="1">
+      <c r="G34" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J34" s="13">
+        <v>1</v>
+      </c>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="1">
+        <v>1</v>
+      </c>
+      <c r="O34" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2323,14 +3283,29 @@
       <c r="F35" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G35" s="1">
-        <v>1</v>
-      </c>
-      <c r="H35" s="1">
+      <c r="G35" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J35" s="13">
+        <v>1</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="1">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2349,14 +3324,29 @@
       <c r="F36" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J36" s="13">
+        <v>3</v>
+      </c>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="1">
         <v>2</v>
       </c>
-      <c r="H36" s="1">
+      <c r="O36" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2375,14 +3365,29 @@
       <c r="F37" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G37" s="1">
-        <v>1</v>
-      </c>
-      <c r="H37" s="1">
+      <c r="G37" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J37" s="13">
+        <v>1</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="1">
+        <v>1</v>
+      </c>
+      <c r="O37" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2401,14 +3406,29 @@
       <c r="F38" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J38" s="13">
+        <v>1</v>
+      </c>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="1">
         <v>2</v>
       </c>
-      <c r="H38" s="1">
+      <c r="O38" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2427,14 +3447,29 @@
       <c r="F39" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G39" s="1">
-        <v>1</v>
-      </c>
-      <c r="H39" s="1">
+      <c r="G39" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J39" s="13">
+        <v>1</v>
+      </c>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="1">
+        <v>1</v>
+      </c>
+      <c r="O39" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2453,14 +3488,29 @@
       <c r="F40" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J40" s="13">
+        <v>1</v>
+      </c>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="1">
         <v>28</v>
       </c>
-      <c r="H40" s="1">
+      <c r="O40" s="1">
         <v>2529</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2479,14 +3529,29 @@
       <c r="F41" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J41" s="13">
+        <v>2</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="1">
         <v>47</v>
       </c>
-      <c r="H41" s="1">
+      <c r="O41" s="1">
         <v>1566</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2505,14 +3570,31 @@
       <c r="F42" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J42" s="13">
+        <v>2</v>
+      </c>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13">
+        <v>3</v>
+      </c>
+      <c r="M42" s="13"/>
+      <c r="N42" s="1">
         <v>172</v>
       </c>
-      <c r="H42" s="1">
+      <c r="O42" s="1">
         <v>5992</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2531,14 +3613,29 @@
       <c r="F43" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G43" s="1">
-        <v>1</v>
-      </c>
-      <c r="H43" s="1">
+      <c r="G43" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J43" s="13">
+        <v>1</v>
+      </c>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="1">
+        <v>1</v>
+      </c>
+      <c r="O43" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2557,14 +3654,29 @@
       <c r="F44" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G44" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J44" s="13">
+        <v>3</v>
+      </c>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="1">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2583,14 +3695,29 @@
       <c r="F45" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G45" s="1">
-        <v>1</v>
-      </c>
-      <c r="H45" s="1">
+      <c r="G45" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J45" s="13">
+        <v>2</v>
+      </c>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="1">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1">
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2609,14 +3736,29 @@
       <c r="F46" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G46" s="1">
-        <v>1</v>
-      </c>
-      <c r="H46" s="1">
+      <c r="G46" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J46" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="1">
+        <v>1</v>
+      </c>
+      <c r="O46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2635,14 +3777,29 @@
       <c r="F47" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G47" s="1">
-        <v>1</v>
-      </c>
-      <c r="H47" s="1">
+      <c r="G47" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J47" s="13">
+        <v>1</v>
+      </c>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="1">
+        <v>1</v>
+      </c>
+      <c r="O47" s="1">
         <v>937</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2661,14 +3818,29 @@
       <c r="F48" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G48" s="1">
-        <v>1</v>
-      </c>
-      <c r="H48" s="1">
+      <c r="G48" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J48" s="13">
+        <v>1</v>
+      </c>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="1">
+        <v>1</v>
+      </c>
+      <c r="O48" s="1">
         <v>867</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2687,14 +3859,29 @@
       <c r="F49" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G49" s="1">
-        <v>1</v>
-      </c>
-      <c r="H49" s="1">
+      <c r="G49" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J49" s="13">
+        <v>1</v>
+      </c>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="1">
+        <v>1</v>
+      </c>
+      <c r="O49" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2713,14 +3900,29 @@
       <c r="F50" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G50" s="1">
-        <v>1</v>
-      </c>
-      <c r="H50" s="1">
+      <c r="G50" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J50" s="13">
+        <v>1</v>
+      </c>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="1">
+        <v>1</v>
+      </c>
+      <c r="O50" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2739,14 +3941,98 @@
       <c r="F51" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G51" s="1">
-        <v>1</v>
-      </c>
-      <c r="H51" s="1">
+      <c r="G51" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J51" s="13">
+        <v>4</v>
+      </c>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="1">
+        <v>1</v>
+      </c>
+      <c r="O51" s="1">
         <v>207</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="67">
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2755,8 +4041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3250ABA8-E85F-4990-9EC1-C50B74D6A166}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2790,10 +4076,10 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -2807,8 +4093,8 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
@@ -2820,8 +4106,8 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
@@ -2833,8 +4119,8 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
@@ -2846,8 +4132,8 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
@@ -2859,10 +4145,10 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -2876,8 +4162,8 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="5" t="s">
         <v>31</v>
       </c>
@@ -2889,8 +4175,8 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="5" t="s">
         <v>33</v>
       </c>
@@ -2902,8 +4188,8 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
@@ -2915,8 +4201,8 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="5" t="s">
         <v>37</v>
       </c>
@@ -2928,8 +4214,8 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="5" t="s">
         <v>39</v>
       </c>
@@ -2941,8 +4227,8 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="5" t="s">
         <v>41</v>
       </c>
@@ -2954,10 +4240,10 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -2971,8 +4257,8 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="5" t="s">
         <v>43</v>
       </c>
@@ -2987,10 +4273,10 @@
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -3018,10 +4304,10 @@
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="19" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -3035,8 +4321,8 @@
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="5" t="s">
         <v>58</v>
       </c>
@@ -3328,13 +4614,13 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="9">
+      <c r="A37" s="20">
         <v>36</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="19" t="s">
         <v>136</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -3345,9 +4631,9 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="8"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="5" t="s">
         <v>251</v>
       </c>
@@ -3356,9 +4642,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="8"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="5" t="s">
         <v>253</v>
       </c>
@@ -3367,9 +4653,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="8"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="5" t="s">
         <v>255</v>
       </c>
@@ -3378,9 +4664,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="8"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="5" t="s">
         <v>259</v>
       </c>
@@ -3389,9 +4675,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="8"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="5" t="s">
         <v>257</v>
       </c>
@@ -3400,9 +4686,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="8"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="5" t="s">
         <v>263</v>
       </c>
@@ -3411,9 +4697,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="8"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="5" t="s">
         <v>261</v>
       </c>
@@ -3422,9 +4708,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="8"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="5" t="s">
         <v>232</v>
       </c>
@@ -3467,13 +4753,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="9">
+      <c r="A48" s="20">
         <v>39</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="19" t="s">
         <v>142</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -3484,9 +4770,9 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="8"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="5" t="s">
         <v>270</v>
       </c>
@@ -3495,9 +4781,9 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="8"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="5" t="s">
         <v>268</v>
       </c>
@@ -3670,13 +4956,13 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="9">
+      <c r="A61" s="20">
         <v>50</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="19" t="s">
         <v>175</v>
       </c>
       <c r="D61" s="5" t="s">
@@ -3687,9 +4973,9 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="8"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="5" t="s">
         <v>289</v>
       </c>
@@ -3698,9 +4984,9 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="8"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="5" t="s">
         <v>285</v>
       </c>
@@ -3709,9 +4995,9 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="8"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="5" t="s">
         <v>283</v>
       </c>
@@ -3720,13 +5006,13 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="9">
+      <c r="A65" s="20">
         <v>51</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="19" t="s">
         <v>179</v>
       </c>
       <c r="D65" s="5" t="s">
@@ -3737,9 +5023,9 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="8"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="5" t="s">
         <v>293</v>
       </c>
@@ -3748,9 +5034,9 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="8"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="19"/>
       <c r="D67" s="5" t="s">
         <v>291</v>
       </c>
@@ -3759,13 +5045,13 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="9">
+      <c r="A68" s="20">
         <v>52</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="19" t="s">
         <v>182</v>
       </c>
       <c r="D68" s="5" t="s">
@@ -3776,9 +5062,9 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="8"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="19"/>
       <c r="D69" s="5" t="s">
         <v>299</v>
       </c>
@@ -3787,9 +5073,9 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="8"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="5" t="s">
         <v>297</v>
       </c>

</xml_diff>